<commit_message>
feat: easy Excel 写入数组字串，使用json转hashmap
</commit_message>
<xml_diff>
--- a/jpa-rest/src/test/resources/template/a.xlsx
+++ b/jpa-rest/src/test/resources/template/a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\java\springboot-all-in-one\jpa-rest\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5546DD8-8753-4C3B-86BA-8909CA356071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92055E0-C76C-4601-B8C7-566ABFAA4950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8234DCBC-DC0D-48A1-BEEF-1E171FB1F3A8}"/>
+    <workbookView xWindow="1608" yWindow="2484" windowWidth="17280" windowHeight="8880" xr2:uid="{8234DCBC-DC0D-48A1-BEEF-1E171FB1F3A8}"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="2" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>nihk</t>
-  </si>
-  <si>
     <t>${customer.name}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -230,6 +227,10 @@
   <si>
     <t>${customer.now}</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{base.name}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -751,7 +752,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -764,7 +765,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -798,16 +799,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -846,20 +847,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f7ac5285-7b0f-47b9-8de3-acca560c2bb8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f7ac5285-7b0f-47b9-8de3-acca560c2bb8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1104,6 +1105,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE460D2-6A27-45AD-A757-26614E63A2A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC05254-FAD5-4313-9C1C-91794A4F8D87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1116,14 +1125,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE460D2-6A27-45AD-A757-26614E63A2A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>